<commit_message>
Copy of competition_players cleaned
</commit_message>
<xml_diff>
--- a/Lorem_datasets/Copy of competition_players(58).xlsx
+++ b/Lorem_datasets/Copy of competition_players(58).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1fbda73f205824d5/Desktop/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\OneDrive\Desktop\Lorem\Lorem_excellentiam\Lorem_datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E4BDE40-6B3C-4348-B55B-19FBFD38A1ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{9E4BDE40-6B3C-4348-B55B-19FBFD38A1ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{060E8B1D-1367-4393-85C7-B55E026D8AEF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{0C8B51FA-6C97-47E2-A4D6-F318C497A32C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{0C8B51FA-6C97-47E2-A4D6-F318C497A32C}"/>
   </bookViews>
   <sheets>
     <sheet name="ref" sheetId="2" r:id="rId1"/>
@@ -10781,7 +10781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168DABA5-1D34-4723-BC18-28D460655C38}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="CU24" sqref="CU24"/>
     </sheetView>
   </sheetViews>
@@ -10936,7 +10936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE7F1DA4-32E7-4134-91E4-3C865B8294C4}">
   <dimension ref="A1:L1942"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -10944,8 +10944,15 @@
   <cols>
     <col min="1" max="1" width="30.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="44.58203125" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.58203125" customWidth="1"/>
+    <col min="3" max="3" width="33.58203125" customWidth="1"/>
+    <col min="4" max="4" width="19.25" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.4140625" customWidth="1"/>
+    <col min="7" max="7" width="19.75" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="26.75" customWidth="1"/>
+    <col min="11" max="11" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>